<commit_message>
Added crit icon on DmgPopup and Hero Inventory
</commit_message>
<xml_diff>
--- a/Assets/HomeAssets/ScriptableObjects/HeroScalings/ClassScalings.xlsx
+++ b/Assets/HomeAssets/ScriptableObjects/HeroScalings/ClassScalings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emaci\Documents\UnityProjects\BrokenHeroes\Assets\HomeAssets\ScriptableObjects\HeroScalings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6D4309-3B2E-4360-BC8F-1E1207D41588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FBDF9C-2573-46D4-AA58-03BCF0E6C7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="120" windowWidth="23232" windowHeight="25296" xr2:uid="{851B7B79-7E9F-4ADA-BC06-EF6855746712}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{851B7B79-7E9F-4ADA-BC06-EF6855746712}"/>
   </bookViews>
   <sheets>
     <sheet name="Scalings" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Class_name</t>
   </si>
   <si>
-    <t>100 * Lvl</t>
-  </si>
-  <si>
     <t>160 * Lvl</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>3 * Lvl / 2</t>
+  </si>
+  <si>
+    <t>90 * Lvl</t>
   </si>
 </sst>
 </file>
@@ -179,9 +179,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -499,10 +498,13 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -534,32 +536,32 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -567,28 +569,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -596,28 +598,28 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -625,28 +627,28 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
         <v>29</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -654,28 +656,28 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -683,28 +685,28 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>